<commit_message>
results of version space
</commit_message>
<xml_diff>
--- a/defect_prediction/27March2015/version_space.xlsx
+++ b/defect_prediction/27March2015/version_space.xlsx
@@ -491,19 +491,19 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.6989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.2959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.7959183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6938775510204"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.79591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.4948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7959183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.7959183673469"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.6989795918367"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4897959183673"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.7959183673469"/>
   </cols>
   <sheetData>

</xml_diff>